<commit_message>
observations on dec 29
</commit_message>
<xml_diff>
--- a/full_exp/blocking.xlsx
+++ b/full_exp/blocking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/seedpriorities/full_exp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF197AF7-6E93-6149-9123-682AECFBBEAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7645C3B1-DC2A-4F41-8BA1-776059220340}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16120" xr2:uid="{ADC4F890-3B43-1949-92D2-2CE1AFFA9832}"/>
   </bookViews>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12226E4A-6B37-0848-9DB2-F55F77AD7E6E}">
-  <dimension ref="A1:B198"/>
+  <dimension ref="A1:B288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="G190" sqref="G190"/>
+    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
+      <selection activeCell="B289" sqref="B289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1983,6 +1983,726 @@
         <v>173</v>
       </c>
     </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>12</v>
+      </c>
+      <c r="B199">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>12</v>
+      </c>
+      <c r="B200">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>12</v>
+      </c>
+      <c r="B201">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>12</v>
+      </c>
+      <c r="B202">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>12</v>
+      </c>
+      <c r="B203">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>12</v>
+      </c>
+      <c r="B204">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>12</v>
+      </c>
+      <c r="B205">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>12</v>
+      </c>
+      <c r="B206">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>12</v>
+      </c>
+      <c r="B207">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>12</v>
+      </c>
+      <c r="B208">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>12</v>
+      </c>
+      <c r="B209">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>12</v>
+      </c>
+      <c r="B210">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>12</v>
+      </c>
+      <c r="B211">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>12</v>
+      </c>
+      <c r="B212">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>12</v>
+      </c>
+      <c r="B213">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>12</v>
+      </c>
+      <c r="B214">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>12</v>
+      </c>
+      <c r="B215">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>12</v>
+      </c>
+      <c r="B216">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>13</v>
+      </c>
+      <c r="B217">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>13</v>
+      </c>
+      <c r="B218">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>13</v>
+      </c>
+      <c r="B219">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>13</v>
+      </c>
+      <c r="B220">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>13</v>
+      </c>
+      <c r="B221">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>13</v>
+      </c>
+      <c r="B222">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>13</v>
+      </c>
+      <c r="B223">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>13</v>
+      </c>
+      <c r="B224">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>13</v>
+      </c>
+      <c r="B225">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>13</v>
+      </c>
+      <c r="B226">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>13</v>
+      </c>
+      <c r="B227">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>13</v>
+      </c>
+      <c r="B228">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>13</v>
+      </c>
+      <c r="B229">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>13</v>
+      </c>
+      <c r="B230">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>13</v>
+      </c>
+      <c r="B231">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>13</v>
+      </c>
+      <c r="B232">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>13</v>
+      </c>
+      <c r="B233">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>13</v>
+      </c>
+      <c r="B234">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>14</v>
+      </c>
+      <c r="B235">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>14</v>
+      </c>
+      <c r="B236">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>14</v>
+      </c>
+      <c r="B237">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>14</v>
+      </c>
+      <c r="B238">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>14</v>
+      </c>
+      <c r="B239">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>14</v>
+      </c>
+      <c r="B240">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>14</v>
+      </c>
+      <c r="B241">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>14</v>
+      </c>
+      <c r="B242">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>14</v>
+      </c>
+      <c r="B243">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>14</v>
+      </c>
+      <c r="B244">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>14</v>
+      </c>
+      <c r="B245">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>14</v>
+      </c>
+      <c r="B246">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>14</v>
+      </c>
+      <c r="B247">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>14</v>
+      </c>
+      <c r="B248">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>14</v>
+      </c>
+      <c r="B249">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>14</v>
+      </c>
+      <c r="B250">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>14</v>
+      </c>
+      <c r="B251">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>14</v>
+      </c>
+      <c r="B252">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>15</v>
+      </c>
+      <c r="B253">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>15</v>
+      </c>
+      <c r="B254">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>15</v>
+      </c>
+      <c r="B255">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>15</v>
+      </c>
+      <c r="B256">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>15</v>
+      </c>
+      <c r="B257">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>15</v>
+      </c>
+      <c r="B258">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>15</v>
+      </c>
+      <c r="B259">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>15</v>
+      </c>
+      <c r="B260">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>15</v>
+      </c>
+      <c r="B261">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>15</v>
+      </c>
+      <c r="B262">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>15</v>
+      </c>
+      <c r="B263">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>15</v>
+      </c>
+      <c r="B264">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>15</v>
+      </c>
+      <c r="B265">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>15</v>
+      </c>
+      <c r="B266">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>15</v>
+      </c>
+      <c r="B267">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>15</v>
+      </c>
+      <c r="B268">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>15</v>
+      </c>
+      <c r="B269">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>15</v>
+      </c>
+      <c r="B270">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>16</v>
+      </c>
+      <c r="B271">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>16</v>
+      </c>
+      <c r="B272">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>16</v>
+      </c>
+      <c r="B273">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>16</v>
+      </c>
+      <c r="B274">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>16</v>
+      </c>
+      <c r="B275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>16</v>
+      </c>
+      <c r="B276">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>16</v>
+      </c>
+      <c r="B277">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>16</v>
+      </c>
+      <c r="B278">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>16</v>
+      </c>
+      <c r="B279">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>16</v>
+      </c>
+      <c r="B280">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>16</v>
+      </c>
+      <c r="B281">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>16</v>
+      </c>
+      <c r="B282">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>16</v>
+      </c>
+      <c r="B283">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>16</v>
+      </c>
+      <c r="B284">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>16</v>
+      </c>
+      <c r="B285">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>16</v>
+      </c>
+      <c r="B286">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <v>16</v>
+      </c>
+      <c r="B287">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>16</v>
+      </c>
+      <c r="B288">
+        <v>245</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>